<commit_message>
Updates to Activity content and Timers
- Resolved issue #2 in debugging report
- Found issue #3, unresolved
- Added content to several Activities to flesh out the app for upcoming peer review
- Updated timer functionality to run better (and not loop beeps when it shouldn't)
</commit_message>
<xml_diff>
--- a/MuayThaiAthletesGuide/MuayThaiAthletesGuide_BugDatabase.xlsx
+++ b/MuayThaiAthletesGuide/MuayThaiAthletesGuide_BugDatabase.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19126"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rachel\Project_MTAG_RachelSoderberg\MuayThaiAthletesGuide\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9276411A-CBAF-4106-B2BA-E0E18DB6282F}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3AD384AD-78A4-4200-98EF-1B2F0D6FCEE3}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9048" xr2:uid="{7AD046E2-E615-4958-9370-F5D8C6562509}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="17">
   <si>
     <t>Steps to Reproduce</t>
   </si>
@@ -60,13 +60,22 @@
     <t>Muay Thai Athletes Guide (MTAG) - Bug Database</t>
   </si>
   <si>
-    <t>User spinner to choose between time cap selections.</t>
-  </si>
-  <si>
     <t>Time cap reflects the correct number of seconds</t>
   </si>
   <si>
     <t>Time cap is not reflecting correct time, instead the preceding or following time cap is given</t>
+  </si>
+  <si>
+    <t>Attempt to run Countdown timer with any time cap</t>
+  </si>
+  <si>
+    <t>Timer should countdown from cap to 0:00</t>
+  </si>
+  <si>
+    <t>User spinner to choose between time cap selections</t>
+  </si>
+  <si>
+    <t>Timer does not countdown correctly, instead it simply ticks down one second and stops</t>
   </si>
 </sst>
 </file>
@@ -142,7 +151,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -165,11 +174,14 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="49" fontId="1" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -488,7 +500,7 @@
   <dimension ref="A1:F15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -503,13 +515,13 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" s="4"/>
-      <c r="B1" s="8" t="s">
+      <c r="B1" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="C1" s="8"/>
-      <c r="D1" s="8"/>
-      <c r="E1" s="8"/>
-      <c r="F1" s="8"/>
+      <c r="C1" s="10"/>
+      <c r="D1" s="10"/>
+      <c r="E1" s="10"/>
+      <c r="F1" s="10"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
@@ -547,33 +559,43 @@
       <c r="E3" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="F3" s="9"/>
+      <c r="F3" s="8"/>
     </row>
     <row r="4" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A4" s="6">
         <v>2</v>
       </c>
       <c r="B4" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C4" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="D4" s="2" t="s">
         <v>12</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>13</v>
       </c>
       <c r="E4" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="F4" s="3"/>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A5" s="6"/>
-      <c r="B5" s="2"/>
-      <c r="C5" s="2"/>
-      <c r="D5" s="2"/>
-      <c r="E5" s="7"/>
-      <c r="F5" s="2"/>
+      <c r="F4" s="9"/>
+    </row>
+    <row r="5" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A5" s="6">
+        <v>3</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="E5" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="F5" s="3"/>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" s="6"/>

</xml_diff>